<commit_message>
Re-run SGNN to annotate dialog acts following clean up work to the original transcripts.
</commit_message>
<xml_diff>
--- a/data/Subset1_WithDialogActs/7th grade math.xlsx_with_dialog_acts.xlsx
+++ b/data/Subset1_WithDialogActs/7th grade math.xlsx_with_dialog_acts.xlsx
@@ -585,12 +585,12 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>sv</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Statement-non-opinion</t>
+          <t>Statement-opinion</t>
         </is>
       </c>
     </row>
@@ -623,12 +623,12 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -737,12 +737,12 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>sv</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Statement-non-opinion</t>
+          <t>Statement-opinion</t>
         </is>
       </c>
     </row>
@@ -775,12 +775,12 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -851,12 +851,12 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -927,12 +927,12 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -1041,12 +1041,12 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>b</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Acknowledge (Backchannel)</t>
         </is>
       </c>
     </row>
@@ -1231,12 +1231,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Statement-non-opinion</t>
+          <t>Agree/Accept</t>
         </is>
       </c>
     </row>
@@ -1345,12 +1345,12 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -1573,12 +1573,12 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -1649,12 +1649,12 @@
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -1839,12 +1839,12 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -2105,12 +2105,12 @@
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -2295,12 +2295,12 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>b</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Acknowledge (Backchannel)</t>
         </is>
       </c>
     </row>
@@ -2409,12 +2409,12 @@
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Statement-non-opinion</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -2485,12 +2485,12 @@
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Agree/Accept</t>
         </is>
       </c>
     </row>
@@ -2637,12 +2637,12 @@
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Agree/Accept</t>
         </is>
       </c>
     </row>
@@ -2713,12 +2713,12 @@
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>sv</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Statement-non-opinion</t>
+          <t>Statement-opinion</t>
         </is>
       </c>
     </row>
@@ -2827,12 +2827,12 @@
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -3549,12 +3549,12 @@
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>b</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Acknowledge (Backchannel)</t>
         </is>
       </c>
     </row>
@@ -3663,12 +3663,12 @@
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -3853,12 +3853,12 @@
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>sv</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Statement-opinion</t>
         </is>
       </c>
     </row>
@@ -3929,12 +3929,12 @@
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -3967,12 +3967,12 @@
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
-          <t>sv</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Statement-opinion</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -4005,12 +4005,12 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -4157,12 +4157,12 @@
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -4195,12 +4195,12 @@
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -4765,12 +4765,12 @@
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>%</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Statement-non-opinion</t>
+          <t>Uninterpretable</t>
         </is>
       </c>
     </row>
@@ -5069,12 +5069,12 @@
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>b</t>
         </is>
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Acknowledge (Backchannel)</t>
         </is>
       </c>
     </row>
@@ -5221,12 +5221,12 @@
       <c r="H126" t="inlineStr"/>
       <c r="I126" t="inlineStr">
         <is>
-          <t>sv</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>Statement-opinion</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -5335,12 +5335,12 @@
       <c r="H129" t="inlineStr"/>
       <c r="I129" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -5487,12 +5487,12 @@
       <c r="H133" t="inlineStr"/>
       <c r="I133" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>
@@ -5563,12 +5563,12 @@
       <c r="H135" t="inlineStr"/>
       <c r="I135" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>Agree/Accept</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -5639,12 +5639,12 @@
       <c r="H137" t="inlineStr"/>
       <c r="I137" t="inlineStr">
         <is>
-          <t>%</t>
+          <t>sd</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>Uninterpretable</t>
+          <t>Statement-non-opinion</t>
         </is>
       </c>
     </row>
@@ -5867,12 +5867,12 @@
       <c r="H143" t="inlineStr"/>
       <c r="I143" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>Acknowledge (Backchannel)</t>
+          <t>Appreciation</t>
         </is>
       </c>
     </row>

</xml_diff>